<commit_message>
workbook: add support for default format
Allow the user to define the default/body format. This
requires that the object positioning code takes the
changed column/row dimensions into account.

Feature #1163
</commit_message>
<xml_diff>
--- a/xlsxwriter/test/comparison/xlsx_files/default_format01.xlsx
+++ b/xlsxwriter/test/comparison/xlsx_files/default_format01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -53,6 +53,49 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="red.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="1524000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -344,8 +387,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>